<commit_message>
CSV Files Created to be Used in Database
This build of the Practice Database files include 'CSV' files which have been prepared to be uploaded to a database in the future.
</commit_message>
<xml_diff>
--- a/2019_game_data_05.xlsx
+++ b/2019_game_data_05.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\COM201\91892_Databases\91892-database-practice-grocottk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E91FA4B-DD13-425E-AC37-2577621FD585}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BB9CCD-CDA1-44BC-9794-9731C9F42831}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="2505" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14865" yWindow="11925" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="6" r:id="rId1"/>
@@ -16025,7 +16025,7 @@
   <dimension ref="A1:L445"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45367,1577 +45367,1577 @@
   <dimension ref="A1:B196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>1410</v>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9">
         <v>1.1100000000000001</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>700</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>468</v>
       </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>443</v>
       </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>452</v>
       </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>596</v>
       </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="B12">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="B14">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="B15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109">
         <v>108</v>
       </c>
-      <c r="B16">
+      <c r="B109" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" s="8" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" s="8" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" s="8" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" s="8" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130" s="8" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132" s="8" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135" s="8" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137" s="8" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138" s="8" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141" s="8" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142" s="8" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143" s="8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144" s="8" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145" s="8" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146" s="8" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147" s="8" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149" s="8" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150" s="8" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151" s="8" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>646</v>
-      </c>
-      <c r="B17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="B19">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="B153" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="B154" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155" s="8" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>155</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>711</v>
-      </c>
-      <c r="B20">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>611</v>
-      </c>
-      <c r="B21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>757</v>
-      </c>
-      <c r="B22">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B23">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B24">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B25">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>352</v>
-      </c>
-      <c r="B26">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="B158" s="8" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>158</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>159</v>
+      </c>
+      <c r="B160" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161" s="8" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>161</v>
+      </c>
+      <c r="B162" s="8" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>162</v>
+      </c>
+      <c r="B163" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>163</v>
+      </c>
+      <c r="B164" s="8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>164</v>
+      </c>
+      <c r="B165" s="8" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>165</v>
+      </c>
+      <c r="B166" s="8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>166</v>
+      </c>
+      <c r="B167" s="8" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>167</v>
+      </c>
+      <c r="B168" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>168</v>
+      </c>
+      <c r="B169" s="8" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>169</v>
+      </c>
+      <c r="B170" s="8" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>170</v>
+      </c>
+      <c r="B171" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>342</v>
-      </c>
-      <c r="B27">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>630</v>
-      </c>
-      <c r="B29">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="B30">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="B31">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>607</v>
-      </c>
-      <c r="B32">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B33">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>739</v>
-      </c>
-      <c r="B34">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B35">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="B36">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>263</v>
-      </c>
-      <c r="B37">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>592</v>
-      </c>
-      <c r="B38">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B39">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B40">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B41">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
-        <v>724</v>
-      </c>
-      <c r="B42">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="B43">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="B44">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
-        <v>514</v>
-      </c>
-      <c r="B45">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>171</v>
+      </c>
+      <c r="B172" s="8" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>172</v>
+      </c>
+      <c r="B173" s="8" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>173</v>
+      </c>
+      <c r="B174" s="8" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>174</v>
+      </c>
+      <c r="B175" s="8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>175</v>
+      </c>
+      <c r="B176" s="8" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>176</v>
+      </c>
+      <c r="B177" s="8" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>177</v>
+      </c>
+      <c r="B178" s="8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>178</v>
+      </c>
+      <c r="B179" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>179</v>
+      </c>
+      <c r="B180" s="8" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>180</v>
+      </c>
+      <c r="B181" s="8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>181</v>
+      </c>
+      <c r="B182" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>182</v>
+      </c>
+      <c r="B183" s="8" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>183</v>
+      </c>
+      <c r="B184" s="8" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>184</v>
+      </c>
+      <c r="B185" s="8" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>185</v>
+      </c>
+      <c r="B186" s="8" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>186</v>
+      </c>
+      <c r="B187" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
-        <v>476</v>
-      </c>
-      <c r="B46">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B47">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="B48">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
-        <v>831</v>
-      </c>
-      <c r="B49">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="B50">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="B51">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
-        <v>496</v>
-      </c>
-      <c r="B52">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B53">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
-        <v>880</v>
-      </c>
-      <c r="B54">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B55">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B56">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="8" t="s">
-        <v>522</v>
-      </c>
-      <c r="B57">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
-        <v>518</v>
-      </c>
-      <c r="B58">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="B59">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B60">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="B61">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="B62">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="8" t="s">
-        <v>486</v>
-      </c>
-      <c r="B63">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="8" t="s">
-        <v>504</v>
-      </c>
-      <c r="B64">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="8" t="s">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>187</v>
+      </c>
+      <c r="B188" s="8" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>188</v>
+      </c>
+      <c r="B189" s="8" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>189</v>
+      </c>
+      <c r="B190" s="8" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191">
         <v>190</v>
       </c>
-      <c r="B65">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B66">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="8" t="s">
-        <v>472</v>
-      </c>
-      <c r="B67">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="8" t="s">
-        <v>665</v>
-      </c>
-      <c r="B68">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="B69">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B70">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B71">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B72">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="8" t="s">
-        <v>551</v>
-      </c>
-      <c r="B73">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="8" t="s">
-        <v>752</v>
-      </c>
-      <c r="B74">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="8" t="s">
-        <v>805</v>
-      </c>
-      <c r="B75">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B76">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="8" t="s">
-        <v>777</v>
-      </c>
-      <c r="B77">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="B78">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="8" t="s">
-        <v>809</v>
-      </c>
-      <c r="B79">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="B80">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="B81">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="8" t="s">
-        <v>678</v>
-      </c>
-      <c r="B82">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="8" t="s">
-        <v>392</v>
-      </c>
-      <c r="B83">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="B84">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="8" t="s">
-        <v>787</v>
-      </c>
-      <c r="B85">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="B86">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="8" t="s">
-        <v>485</v>
-      </c>
-      <c r="B87">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="B88">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B89">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="8" t="s">
-        <v>615</v>
-      </c>
-      <c r="B90">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="B91">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="8" t="s">
-        <v>394</v>
-      </c>
-      <c r="B92">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="B93">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="8" t="s">
-        <v>851</v>
-      </c>
-      <c r="B94">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B95">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="8" t="s">
-        <v>795</v>
-      </c>
-      <c r="B96">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="8" t="s">
-        <v>451</v>
-      </c>
-      <c r="B97">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="8" t="s">
-        <v>289</v>
-      </c>
-      <c r="B98">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="8" t="s">
-        <v>817</v>
-      </c>
-      <c r="B99">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="8" t="s">
-        <v>564</v>
-      </c>
-      <c r="B100">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="8" t="s">
-        <v>619</v>
-      </c>
-      <c r="B101">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="8" t="s">
-        <v>791</v>
-      </c>
-      <c r="B102">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="8" t="s">
-        <v>433</v>
-      </c>
-      <c r="B103">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="8" t="s">
-        <v>802</v>
-      </c>
-      <c r="B104">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="8" t="s">
-        <v>824</v>
-      </c>
-      <c r="B105">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="8" t="s">
-        <v>861</v>
-      </c>
-      <c r="B106">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="8" t="s">
-        <v>753</v>
-      </c>
-      <c r="B107">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B108">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B109">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="B110">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="8" t="s">
-        <v>674</v>
-      </c>
-      <c r="B111">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="B112">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="8" t="s">
-        <v>669</v>
-      </c>
-      <c r="B113">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="8" t="s">
-        <v>456</v>
-      </c>
-      <c r="B114">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B115">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="8" t="s">
-        <v>465</v>
-      </c>
-      <c r="B116">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="B117">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B118">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B119">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="8" t="s">
-        <v>457</v>
-      </c>
-      <c r="B120">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="8" t="s">
-        <v>571</v>
-      </c>
-      <c r="B121">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="B122">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="8" t="s">
-        <v>391</v>
-      </c>
-      <c r="B123">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="8" t="s">
-        <v>544</v>
-      </c>
-      <c r="B124">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="B125">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B126">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="8" t="s">
-        <v>414</v>
-      </c>
-      <c r="B127">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="8" t="s">
-        <v>838</v>
-      </c>
-      <c r="B128">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="8" t="s">
-        <v>687</v>
-      </c>
-      <c r="B129">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="B130">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="B131">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="8" t="s">
-        <v>636</v>
-      </c>
-      <c r="B132">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B133">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="B134">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="8" t="s">
-        <v>477</v>
-      </c>
-      <c r="B135">
+      <c r="B191" s="8" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>191</v>
+      </c>
+      <c r="B192" s="8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>192</v>
+      </c>
+      <c r="B193" s="8" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>193</v>
+      </c>
+      <c r="B194" s="8" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="B136">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="8" t="s">
-        <v>464</v>
-      </c>
-      <c r="B137">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="8" t="s">
-        <v>401</v>
-      </c>
-      <c r="B138">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="B139">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B140">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="8" t="s">
-        <v>500</v>
-      </c>
-      <c r="B141">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="B142">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="B143">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="8" t="s">
-        <v>427</v>
-      </c>
-      <c r="B144">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="8" t="s">
-        <v>541</v>
-      </c>
-      <c r="B145">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="8" t="s">
-        <v>650</v>
-      </c>
-      <c r="B146">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="8" t="s">
-        <v>897</v>
-      </c>
-      <c r="B147">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B148">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="8" t="s">
-        <v>410</v>
-      </c>
-      <c r="B149">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="8" t="s">
-        <v>405</v>
-      </c>
-      <c r="B150">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="8" t="s">
-        <v>553</v>
-      </c>
-      <c r="B151">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B152">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B153">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="B154">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="8" t="s">
-        <v>330</v>
-      </c>
-      <c r="B155">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="B156">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B157">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="8" t="s">
-        <v>600</v>
-      </c>
-      <c r="B158">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="B159">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B160">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="8" t="s">
-        <v>588</v>
-      </c>
-      <c r="B161">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="8" t="s">
-        <v>560</v>
-      </c>
-      <c r="B162">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B163">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="B164">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="B165">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="B166">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="8" t="s">
-        <v>708</v>
-      </c>
-      <c r="B167">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B168">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="8" t="s">
-        <v>384</v>
-      </c>
-      <c r="B169">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" s="8" t="s">
-        <v>813</v>
-      </c>
-      <c r="B170">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B171">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="B172">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="8" t="s">
-        <v>510</v>
-      </c>
-      <c r="B173">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="8" t="s">
-        <v>735</v>
-      </c>
-      <c r="B174">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="B175">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" s="8" t="s">
-        <v>773</v>
-      </c>
-      <c r="B176">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="B177">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="B178">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="B179">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" s="8" t="s">
-        <v>447</v>
-      </c>
-      <c r="B180">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="B181">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="B182">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="8" t="s">
-        <v>642</v>
-      </c>
-      <c r="B183">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" s="8" t="s">
-        <v>626</v>
-      </c>
-      <c r="B184">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" s="8" t="s">
-        <v>557</v>
-      </c>
-      <c r="B185">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" s="8" t="s">
-        <v>420</v>
-      </c>
-      <c r="B186">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B187">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" s="8" t="s">
-        <v>783</v>
-      </c>
-      <c r="B188">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="8" t="s">
-        <v>534</v>
-      </c>
-      <c r="B189">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A190" s="8" t="s">
-        <v>552</v>
-      </c>
-      <c r="B190">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="B191">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="B192">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" s="8" t="s">
-        <v>578</v>
-      </c>
-      <c r="B193">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B194">
-        <v>193</v>
-      </c>
-    </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A195" s="8" t="s">
+      <c r="A195">
+        <v>194</v>
+      </c>
+      <c r="B195" s="8" t="s">
         <v>728</v>
       </c>
-      <c r="B195">
-        <v>194</v>
-      </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A196" s="8"/>
+      <c r="B196" s="8"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A445">
-    <sortCondition ref="A2:A445"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B445">
+    <sortCondition ref="B2:B445"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -46948,150 +46948,153 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B1" t="s">
         <v>878</v>
       </c>
-      <c r="B1" t="s">
-        <v>1409</v>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>882</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>981</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>881</v>
       </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>976</v>
       </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>978</v>
       </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>984</v>
       </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>982</v>
       </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>980</v>
       </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>979</v>
       </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>983</v>
       </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>701</v>
       </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>985</v>
       </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>977</v>
       </c>
-      <c r="B14">
-        <v>13</v>
-      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>879</v>
       </c>
-      <c r="B15">
-        <v>14</v>
-      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>986</v>
       </c>
-      <c r="B16">
-        <v>15</v>
-      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>987</v>
       </c>
-      <c r="B17">
-        <v>16</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A444">
-    <sortCondition ref="A2:A444"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B444">
+    <sortCondition ref="B2:B444"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>